<commit_message>
Updated Cost Analysis.pdf, Cost Budget Estimate.pdf, & Cost Budget Estimate.xlsx
</commit_message>
<xml_diff>
--- a/documentation/projman/Cost Budget Estimate.xlsx
+++ b/documentation/projman/Cost Budget Estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\APC_2022_2023_T3_PROJMAN_MI201_MI203_G03_Team_MLNSD\documentation\projman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3598DDFF-62B9-4643-8B7E-08F8C9A83AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A8A58C-8665-4BCE-B477-E35E8E4684CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -128,9 +128,6 @@
     <t>Actual Cost</t>
   </si>
   <si>
-    <t>Rental (10% of Depreciated Value)</t>
-  </si>
-  <si>
     <t>Web Hosting (GoDaddy)</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>Domain Registration  (GoDaddy)</t>
+  </si>
+  <si>
+    <t>Rental Rate</t>
   </si>
 </sst>
 </file>
@@ -352,17 +352,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -370,23 +368,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,13 +416,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -735,10 +736,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -753,369 +754,372 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="4">
         <f>SUM(F6:F7,F10:F18)</f>
-        <v>2338085.8199999998</v>
+        <v>2342335.8199999998</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6">
+      <c r="F1" s="5">
         <f>296+181</f>
         <v>477</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="28"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <f>(296+181)*9</f>
         <v>4293</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>100</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <f>C6*B6</f>
         <v>429300</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>5</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <f>D6*E6</f>
         <v>2146500</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <f>181*9</f>
         <v>1629</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>100</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <f>C7*B7</f>
         <v>162900</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="9">
         <f>D7*E7</f>
         <v>162900</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="11"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="19"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="8" t="s">
+      <c r="C10" s="17">
+        <v>5988</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="16">
+        <v>5988</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="31">
-        <v>5988</v>
-      </c>
-      <c r="D10" s="20">
+      <c r="C11" s="17">
+        <v>7999</v>
+      </c>
+      <c r="D11" s="15">
         <v>1</v>
       </c>
-      <c r="E10" s="18"/>
-      <c r="F10" s="21">
-        <v>5988</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="8" t="s">
+      <c r="E11" s="32"/>
+      <c r="F11" s="16">
+        <v>7999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="31">
-        <v>7999</v>
-      </c>
-      <c r="D11" s="20">
+      <c r="C12" s="17">
+        <v>998.82</v>
+      </c>
+      <c r="D12" s="15">
         <v>1</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="21">
-        <v>7999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="31">
+      <c r="E12" s="32"/>
+      <c r="F12" s="16">
         <v>998.82</v>
       </c>
-      <c r="D12" s="20">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="17">
+        <v>35500</v>
+      </c>
+      <c r="D13" s="15">
+        <v>2</v>
+      </c>
+      <c r="E13" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="F13" s="16">
+        <f>(C13-(C13*(D13*0.2)))*E13</f>
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="17">
+        <v>50000</v>
+      </c>
+      <c r="D14" s="15">
+        <v>3</v>
+      </c>
+      <c r="E14" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="F14" s="16">
+        <f>(C14-(C14*(D14*0.2)))*E14</f>
+        <v>1999.9999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="17">
+        <v>44000</v>
+      </c>
+      <c r="D15" s="15">
+        <v>3</v>
+      </c>
+      <c r="E15" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="F15" s="16">
+        <f>(C15-(C15*(D15*0.2)))*E15</f>
+        <v>1759.9999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="17">
+        <v>50000</v>
+      </c>
+      <c r="D16" s="15">
+        <v>2</v>
+      </c>
+      <c r="E16" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="F16" s="16">
+        <f>(C16-(C16*(D16*0.2)))*E16</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="17">
+        <v>95000</v>
+      </c>
+      <c r="D17" s="15">
+        <v>2</v>
+      </c>
+      <c r="E17" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="F17" s="16">
+        <f>(C17-(C17*(D17*0.2)))*E17</f>
+        <v>5700</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="18">
+        <v>42000</v>
+      </c>
+      <c r="D18" s="15">
         <v>1</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="21">
-        <v>998.82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="31">
-        <v>35500</v>
-      </c>
-      <c r="D13" s="20">
-        <v>2</v>
-      </c>
-      <c r="E13" s="33">
-        <f>(C13-(C13*(D13*0.2)))*0.1</f>
-        <v>2130</v>
-      </c>
-      <c r="F13" s="21">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="31">
-        <v>50000</v>
-      </c>
-      <c r="D14" s="20">
-        <v>3</v>
-      </c>
-      <c r="E14" s="33">
-        <f>(C14-(C14*(D14*0.2)))*0.1</f>
-        <v>1999.9999999999998</v>
-      </c>
-      <c r="F14" s="21">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="31">
-        <v>44000</v>
-      </c>
-      <c r="D15" s="20">
-        <v>3</v>
-      </c>
-      <c r="E15" s="33">
-        <f>(C15-(C15*(D15*0.2)))*0.1</f>
-        <v>1759.9999999999998</v>
-      </c>
-      <c r="F15" s="21">
-        <v>2640</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A16" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="31">
-        <v>50000</v>
-      </c>
-      <c r="D16" s="20">
-        <v>2</v>
-      </c>
-      <c r="E16" s="33">
-        <f>(C16-(C16*(D16*0.2)))*0.1</f>
-        <v>3000</v>
-      </c>
-      <c r="F16" s="21">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="31">
-        <v>95000</v>
-      </c>
-      <c r="D17" s="20">
-        <v>2</v>
-      </c>
-      <c r="E17" s="33">
-        <f>(C17-(C17*(D17*0.2)))*0.1</f>
-        <v>5700</v>
-      </c>
-      <c r="F17" s="21">
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="32">
-        <v>42000</v>
-      </c>
-      <c r="D18" s="20">
-        <v>1</v>
-      </c>
-      <c r="E18" s="33">
-        <f>(C18-(C18*(D18*0.2)))*0.1</f>
+      <c r="E18" s="32">
+        <v>0.1</v>
+      </c>
+      <c r="F18" s="16">
+        <f>(C18-(C18*(D18*0.2)))*E18</f>
         <v>3360</v>
       </c>
-      <c r="F18" s="21">
-        <v>840</v>
-      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="11"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="19"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="8"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Update Cost Budget Estimate.xlsx & Cost Management Plan_MLNSD.docx
</commit_message>
<xml_diff>
--- a/documentation/projman/Cost Budget Estimate.xlsx
+++ b/documentation/projman/Cost Budget Estimate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\APC_2022_2023_T3_PROJMAN_MI201_MI203_G03_Team_MLNSD\documentation\projman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A8A58C-8665-4BCE-B477-E35E8E4684CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA1F395-9498-4F5C-B789-B3859949F67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>Total Cost</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>Rental Rate</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Product Owner</t>
   </si>
 </sst>
 </file>
@@ -192,7 +198,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -349,6 +355,24 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -357,7 +381,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -377,46 +401,81 @@
     <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -736,10 +795,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -753,12 +812,12 @@
     <col min="7" max="7" width="13.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4">
-        <f>SUM(F6:F7,F10:F18)</f>
+        <f>SUM(F6:F9,F12:F20)</f>
         <v>2342335.8199999998</v>
       </c>
       <c r="C1" s="2"/>
@@ -771,35 +830,35 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="29" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -819,7 +878,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -835,14 +894,14 @@
         <v>429300</v>
       </c>
       <c r="E6" s="7">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F6" s="9">
         <f>D6*E6</f>
-        <v>2146500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+        <v>1287900</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -865,172 +924,179 @@
         <v>162900</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <f>B6</f>
+        <v>4293</v>
+      </c>
+      <c r="C8" s="7">
+        <v>100</v>
+      </c>
+      <c r="D8" s="41">
+        <f>B8*C8</f>
+        <v>429300</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <f>E8*D8</f>
+        <v>429300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <f>B8</f>
+        <v>4293</v>
+      </c>
+      <c r="C9" s="7">
+        <v>100</v>
+      </c>
+      <c r="D9" s="41">
+        <f>C9*B9</f>
+        <v>429300</v>
+      </c>
+      <c r="E9" s="42">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <f>E9*D9</f>
+        <v>429300</v>
+      </c>
+      <c r="I9">
+        <v>2342335.8199999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="19"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="6" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="17">
-        <v>5988</v>
-      </c>
-      <c r="D10" s="15">
-        <v>1</v>
-      </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="16">
-        <v>5988</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="17">
-        <v>7999</v>
-      </c>
-      <c r="D11" s="15">
-        <v>1</v>
-      </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="16">
-        <v>7999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" s="17">
-        <v>998.82</v>
+        <v>5988</v>
       </c>
       <c r="D12" s="15">
         <v>1</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="16">
+        <v>5988</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="17">
+        <v>7999</v>
+      </c>
+      <c r="D13" s="15">
+        <v>1</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="16">
+        <v>7999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="17">
         <v>998.82</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="17">
-        <v>35500</v>
-      </c>
-      <c r="D13" s="15">
-        <v>2</v>
-      </c>
-      <c r="E13" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="F13" s="16">
-        <f>(C13-(C13*(D13*0.2)))*E13</f>
-        <v>2130</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="17">
-        <v>50000</v>
-      </c>
       <c r="D14" s="15">
-        <v>3</v>
-      </c>
-      <c r="E14" s="32">
-        <v>0.1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E14" s="19"/>
       <c r="F14" s="16">
-        <f>(C14-(C14*(D14*0.2)))*E14</f>
-        <v>1999.9999999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+        <v>998.82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C15" s="17">
-        <v>44000</v>
+        <v>35500</v>
       </c>
       <c r="D15" s="15">
-        <v>3</v>
-      </c>
-      <c r="E15" s="32">
+        <v>2</v>
+      </c>
+      <c r="E15" s="19">
         <v>0.1</v>
       </c>
       <c r="F15" s="16">
-        <f>(C15-(C15*(D15*0.2)))*E15</f>
-        <v>1759.9999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+        <f t="shared" ref="F15:F20" si="0">(C15-(C15*(D15*0.2)))*E15</f>
+        <v>2130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C16" s="17">
         <v>50000</v>
       </c>
       <c r="D16" s="15">
-        <v>2</v>
-      </c>
-      <c r="E16" s="32">
+        <v>3</v>
+      </c>
+      <c r="E16" s="19">
         <v>0.1</v>
       </c>
       <c r="F16" s="16">
-        <f>(C16-(C16*(D16*0.2)))*E16</f>
-        <v>3000</v>
+        <f t="shared" si="0"/>
+        <v>1999.9999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -1038,20 +1104,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17" s="17">
-        <v>95000</v>
+        <v>44000</v>
       </c>
       <c r="D17" s="15">
-        <v>2</v>
-      </c>
-      <c r="E17" s="32">
+        <v>3</v>
+      </c>
+      <c r="E17" s="19">
         <v>0.1</v>
       </c>
       <c r="F17" s="16">
-        <f>(C17-(C17*(D17*0.2)))*E17</f>
-        <v>5700</v>
+        <f t="shared" si="0"/>
+        <v>1759.9999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -1059,73 +1125,110 @@
         <v>16</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="18">
-        <v>42000</v>
+        <v>19</v>
+      </c>
+      <c r="C18" s="17">
+        <v>50000</v>
       </c>
       <c r="D18" s="15">
-        <v>1</v>
-      </c>
-      <c r="E18" s="32">
+        <v>2</v>
+      </c>
+      <c r="E18" s="19">
         <v>0.1</v>
       </c>
       <c r="F18" s="16">
-        <f>(C18-(C18*(D18*0.2)))*E18</f>
-        <v>3360</v>
+        <f t="shared" si="0"/>
+        <v>3000</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="19"/>
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="17">
+        <v>95000</v>
+      </c>
+      <c r="D19" s="15">
+        <v>2</v>
+      </c>
+      <c r="E19" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="0"/>
+        <v>5700</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="18">
+        <v>42000</v>
+      </c>
+      <c r="D20" s="15">
+        <v>1</v>
+      </c>
+      <c r="E20" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="16">
+        <f t="shared" si="0"/>
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="40"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B22" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="7" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="31"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="7"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A24" s="7"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
       <c r="G24" s="1"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="F25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A19:F19"/>
-    <mergeCell ref="B20:F22"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="B22:F24"/>
     <mergeCell ref="A2:F3"/>
     <mergeCell ref="A4:F4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updated Cost Budget Estimate.xlsx && Added Salary Reference (Full Stack Web Developer)_Web Developer (Full Stack) - Pasig - Indeed.com.pdf && Added Salary Reference (Product Owner)_Product Owner - Makati - Indeed.com.pdf
</commit_message>
<xml_diff>
--- a/documentation/projman/Cost Budget Estimate.xlsx
+++ b/documentation/projman/Cost Budget Estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\APC_2022_2023_T3_PROJMAN_MI201_MI203_G03_Team_MLNSD\documentation\projman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA1F395-9498-4F5C-B789-B3859949F67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D48A83-D9C5-4A67-AD26-DA6B48164F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
+    <workbookView xWindow="5940" yWindow="1628" windowWidth="14400" windowHeight="7372" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,59 +402,16 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,16 +422,59 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -798,7 +798,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -818,7 +818,7 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(F6:F9,F12:F20)</f>
-        <v>2342335.8199999998</v>
+        <v>3685810.82</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -831,32 +831,32 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
@@ -910,18 +910,18 @@
         <v>1629</v>
       </c>
       <c r="C7" s="7">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D7" s="8">
         <f>C7*B7</f>
-        <v>162900</v>
+        <v>325800</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="9">
         <f>D7*E7</f>
-        <v>162900</v>
+        <v>325800</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -935,7 +935,7 @@
       <c r="C8" s="7">
         <v>100</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="20">
         <f>B8*C8</f>
         <v>429300</v>
       </c>
@@ -956,32 +956,32 @@
         <v>4293</v>
       </c>
       <c r="C9" s="7">
-        <v>100</v>
-      </c>
-      <c r="D9" s="41">
+        <v>375</v>
+      </c>
+      <c r="D9" s="20">
         <f>C9*B9</f>
-        <v>429300</v>
-      </c>
-      <c r="E9" s="42">
+        <v>1609875</v>
+      </c>
+      <c r="E9" s="21">
         <v>1</v>
       </c>
       <c r="F9" s="1">
         <f>E9*D9</f>
-        <v>429300</v>
+        <v>1609875</v>
       </c>
       <c r="I9">
         <v>2342335.8199999998</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="45"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
@@ -1184,44 +1184,44 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
       <c r="G24" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Cost Budget Estimate.xlsx
</commit_message>
<xml_diff>
--- a/documentation/projman/Cost Budget Estimate.xlsx
+++ b/documentation/projman/Cost Budget Estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\APC_2022_2023_T3_PROJMAN_MI201_MI203_G03_Team_MLNSD\documentation\projman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA1F395-9498-4F5C-B789-B3859949F67A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E462731-1505-4B4A-B914-F8A493376EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="14400" windowHeight="7372" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,59 +402,16 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -465,16 +422,59 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -798,7 +798,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -818,7 +818,7 @@
       </c>
       <c r="B1" s="4">
         <f>SUM(F6:F9,F12:F20)</f>
-        <v>2342335.8199999998</v>
+        <v>2423785.8199999998</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -831,32 +831,32 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
@@ -910,18 +910,18 @@
         <v>1629</v>
       </c>
       <c r="C7" s="7">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D7" s="8">
         <f>C7*B7</f>
-        <v>162900</v>
+        <v>244350</v>
       </c>
       <c r="E7" s="7">
         <v>1</v>
       </c>
       <c r="F7" s="9">
         <f>D7*E7</f>
-        <v>162900</v>
+        <v>244350</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -935,7 +935,7 @@
       <c r="C8" s="7">
         <v>100</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D8" s="20">
         <f>B8*C8</f>
         <v>429300</v>
       </c>
@@ -958,11 +958,11 @@
       <c r="C9" s="7">
         <v>100</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D9" s="20">
         <f>C9*B9</f>
         <v>429300</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="21">
         <v>1</v>
       </c>
       <c r="F9" s="1">
@@ -974,14 +974,14 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="45"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="24"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
@@ -1184,44 +1184,44 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="40"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="27"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="31"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="7"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="37"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="36"/>
       <c r="G24" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Cost Budget Estimate(OpenProject).png && Cost Budget Estimate.png
Updated Cost Budget Estimate.xlsx && Cost Management Plan_MLNSD.docx
</commit_message>
<xml_diff>
--- a/documentation/projman/Cost Budget Estimate.xlsx
+++ b/documentation/projman/Cost Budget Estimate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\APC_2022_2023_T3_PROJMAN_MI201_MI203_G03_Team_MLNSD\documentation\projman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C8675F-F09D-468D-A1D5-CF36B1216B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB610096-C7C5-494C-8EA9-47A8A8122AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="14400" windowHeight="7372" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Total Cost</t>
   </si>
   <si>
-    <t>Budget</t>
-  </si>
-  <si>
     <t>Project Duration</t>
   </si>
   <si>
@@ -53,24 +50,15 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>Labor Cost Estimate</t>
   </si>
   <si>
     <t>Hourly Rate</t>
   </si>
   <si>
-    <t>Total Cost (477 days * 9 hours)</t>
-  </si>
-  <si>
     <t>Hours Spent</t>
   </si>
   <si>
-    <t>Quality Asurance</t>
-  </si>
-  <si>
     <t>Developer</t>
   </si>
   <si>
@@ -89,30 +77,9 @@
     <t>Equipment</t>
   </si>
   <si>
-    <t>Laptop (Fia Villamin)</t>
-  </si>
-  <si>
-    <t>Laptop (Dale Joshua)</t>
-  </si>
-  <si>
-    <t>Laptop (Mabelle Aspeli)</t>
-  </si>
-  <si>
-    <t>Laptop (Nathaniel Sison)</t>
-  </si>
-  <si>
-    <t>Laptop (Leigh Camara)</t>
-  </si>
-  <si>
-    <t>Laptop (Ludwig Angeles)</t>
-  </si>
-  <si>
     <t>Subtotal</t>
   </si>
   <si>
-    <t>Duration (Years)</t>
-  </si>
-  <si>
     <t>Utilities</t>
   </si>
   <si>
@@ -125,9 +92,6 @@
     <t>Indirect Cost</t>
   </si>
   <si>
-    <t>Actual Cost</t>
-  </si>
-  <si>
     <t>Web Hosting (GoDaddy)</t>
   </si>
   <si>
@@ -144,15 +108,50 @@
   </si>
   <si>
     <t>Product Owner</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>Quality Asurance (Leigh)</t>
+  </si>
+  <si>
+    <t>Quality Asurance (Ludwig)</t>
+  </si>
+  <si>
+    <t>Laptop (QA)</t>
+  </si>
+  <si>
+    <t>Laptop (Developer)</t>
+  </si>
+  <si>
+    <t>Laptop (Product Owner &amp; Project Manager)</t>
+  </si>
+  <si>
+    <t>Laptop (Tester)</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t>Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;₱&quot;* #,##0.00_-;\-&quot;₱&quot;* #,##0.00_-;_-&quot;₱&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$₱-3409]* #,##0.00_-;\-[$₱-3409]* #,##0.00_-;_-[$₱-3409]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;₱&quot;* #,##0.000_-;\-&quot;₱&quot;* #,##0.000_-;_-&quot;₱&quot;* &quot;-&quot;???_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -381,7 +380,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -390,8 +389,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -403,7 +400,6 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -434,9 +430,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -476,6 +469,30 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -795,16 +812,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D11" sqref="D11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="37.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.53125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.19921875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.796875" bestFit="1" customWidth="1"/>
@@ -814,16 +831,16 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4">
-        <f>SUM(F6:F9,F12:F20)</f>
-        <v>3608653.82</v>
+        <f>SUM(D6:F11,F14:F20)</f>
+        <v>126774.22</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F1" s="5">
         <f>296+181</f>
@@ -831,404 +848,412 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="37" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="39"/>
+      <c r="A2" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="40"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
+      <c r="A4" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="20"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B6" s="7">
-        <f>(296+181)*9</f>
-        <v>4293</v>
+        <v>71</v>
       </c>
       <c r="C6" s="7">
-        <v>192</v>
-      </c>
-      <c r="D6" s="8">
+        <v>120</v>
+      </c>
+      <c r="D6" s="45">
         <f>C6*B6</f>
-        <v>824256</v>
-      </c>
-      <c r="E6" s="7">
-        <v>3</v>
-      </c>
-      <c r="F6" s="9">
-        <f>D6*E6</f>
-        <v>2472768</v>
-      </c>
+        <v>8520</v>
+      </c>
+      <c r="E6" s="46"/>
+      <c r="F6" s="47"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B7" s="7">
-        <f>181*9</f>
-        <v>1629</v>
+        <v>170</v>
       </c>
       <c r="C7" s="7">
-        <v>150</v>
-      </c>
-      <c r="D7" s="8">
+        <v>120</v>
+      </c>
+      <c r="D7" s="45">
         <f>C7*B7</f>
-        <v>244350</v>
-      </c>
-      <c r="E7" s="7">
-        <v>1</v>
-      </c>
-      <c r="F7" s="9">
-        <f>D7*E7</f>
-        <v>244350</v>
-      </c>
+        <v>20400</v>
+      </c>
+      <c r="E7" s="46"/>
+      <c r="F7" s="47"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8">
-        <f>B6</f>
-        <v>4293</v>
+      <c r="A8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7">
+        <v>185</v>
       </c>
       <c r="C8" s="7">
-        <v>100</v>
-      </c>
-      <c r="D8" s="20">
-        <f>B8*C8</f>
-        <v>429300</v>
-      </c>
-      <c r="E8" s="7">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <f>E8*D8</f>
-        <v>429300</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D8" s="45">
+        <f>C8*B8</f>
+        <v>27565</v>
+      </c>
+      <c r="E8" s="46"/>
+      <c r="F8" s="47"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9">
-        <f>B8</f>
-        <v>4293</v>
+      <c r="A9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="7">
+        <v>48</v>
       </c>
       <c r="C9" s="7">
-        <v>100</v>
-      </c>
-      <c r="D9" s="20">
-        <f>C9*B9</f>
-        <v>429300</v>
-      </c>
-      <c r="E9" s="21">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <f>E9*D9</f>
-        <v>429300</v>
-      </c>
+        <v>252</v>
+      </c>
+      <c r="D9" s="48">
+        <f>B9*C9</f>
+        <v>12096</v>
+      </c>
+      <c r="E9" s="49"/>
+      <c r="F9" s="50"/>
       <c r="I9">
         <v>2342335.8199999998</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24"/>
+      <c r="A10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="7">
+        <v>27</v>
+      </c>
+      <c r="C10" s="7">
+        <v>240</v>
+      </c>
+      <c r="D10" s="48">
+        <f>C10*B10</f>
+        <v>6480</v>
+      </c>
+      <c r="E10" s="49"/>
+      <c r="F10" s="50"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="A11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="B11" s="7">
+        <v>60</v>
+      </c>
+      <c r="C11" s="7">
+        <v>268</v>
+      </c>
+      <c r="D11" s="48">
+        <f>C11*B11</f>
+        <v>16080</v>
+      </c>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="17">
-        <v>5988</v>
-      </c>
-      <c r="D12" s="15">
-        <v>1</v>
-      </c>
-      <c r="E12" s="19"/>
-      <c r="F12" s="16">
-        <v>5988</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="17">
-        <v>7999</v>
-      </c>
-      <c r="D13" s="15">
-        <v>1</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="16">
-        <v>7999</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="17">
-        <v>998.82</v>
-      </c>
-      <c r="D14" s="15">
-        <v>1</v>
-      </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="16">
-        <v>998.82</v>
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="15">
+        <v>5988</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="14">
+        <v>5988</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="17">
-        <v>35500</v>
-      </c>
-      <c r="D15" s="15">
-        <v>2</v>
-      </c>
-      <c r="E15" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F15" s="16">
-        <f t="shared" ref="F15:F20" si="0">(C15-(C15*(D15*0.2)))*E15</f>
-        <v>2130</v>
+        <v>11</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="15">
+        <v>7999</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="14">
+        <v>7999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="17">
-        <v>50000</v>
-      </c>
-      <c r="D16" s="15">
-        <v>3</v>
-      </c>
-      <c r="E16" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F16" s="16">
-        <f t="shared" si="0"/>
-        <v>1999.9999999999998</v>
+        <v>11</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="15">
+        <v>998.82</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="14">
+        <v>998.82</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="17">
-        <v>44000</v>
-      </c>
-      <c r="D17" s="15">
-        <v>3</v>
-      </c>
-      <c r="E17" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F17" s="16">
-        <f t="shared" si="0"/>
-        <v>1759.9999999999998</v>
+        <v>12</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="15">
+        <v>20000</v>
+      </c>
+      <c r="D17" s="13">
+        <f>35+47</f>
+        <v>82</v>
+      </c>
+      <c r="E17" s="51">
+        <v>1E-3</v>
+      </c>
+      <c r="F17" s="14">
+        <f t="shared" ref="F17:F18" si="0">(C17*E17)*D17</f>
+        <v>1640</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="17">
-        <v>50000</v>
-      </c>
-      <c r="D18" s="15">
-        <v>2</v>
-      </c>
-      <c r="E18" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F18" s="16">
+        <v>12</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="15">
+        <v>17600</v>
+      </c>
+      <c r="D18" s="13">
+        <v>60</v>
+      </c>
+      <c r="E18" s="51">
+        <v>1E-3</v>
+      </c>
+      <c r="F18" s="14">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="17">
-        <v>95000</v>
-      </c>
-      <c r="D19" s="15">
-        <v>2</v>
-      </c>
-      <c r="E19" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F19" s="16">
-        <f t="shared" si="0"/>
-        <v>5700</v>
+        <v>12</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="15">
+        <v>57000</v>
+      </c>
+      <c r="D19" s="13">
+        <v>177</v>
+      </c>
+      <c r="E19" s="51">
+        <v>1E-3</v>
+      </c>
+      <c r="F19" s="14">
+        <f>(C19*E19)*D19</f>
+        <v>10089</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="18">
-        <v>42000</v>
-      </c>
-      <c r="D20" s="15">
-        <v>1</v>
-      </c>
-      <c r="E20" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="F20" s="16">
-        <f t="shared" si="0"/>
-        <v>3360</v>
+        <v>12</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="16">
+        <v>33600</v>
+      </c>
+      <c r="D20" s="13">
+        <f>162+72</f>
+        <v>234</v>
+      </c>
+      <c r="E20" s="51">
+        <v>1E-3</v>
+      </c>
+      <c r="F20" s="14">
+        <f>(C20*E20)*D20</f>
+        <v>7862.4000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="27"/>
+      <c r="A21" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="24"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="30"/>
+        <v>14</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="27"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="33"/>
+        <v>15</v>
+      </c>
+      <c r="B23" s="28"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="29"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="7"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="1"/>
+      <c r="A24" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="30"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G25" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D27" s="18"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="43"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D28" s="18"/>
+      <c r="E28" s="42"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D29" s="18"/>
+      <c r="E29" s="42"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D30" s="18"/>
+      <c r="E30" s="42"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D31" s="18"/>
+      <c r="E31" s="42"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D32" s="18"/>
+      <c r="E32" s="42"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D33" s="18"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D34" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A10:F10"/>
+  <mergeCells count="12">
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B22:F24"/>
+    <mergeCell ref="A12:F12"/>
     <mergeCell ref="A21:F21"/>
-    <mergeCell ref="B22:F24"/>
     <mergeCell ref="A2:F3"/>
     <mergeCell ref="A4:F4"/>
   </mergeCells>

</xml_diff>